<commit_message>
add easynetq stats to spreadsheet for durable
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="stats" sheetId="1" r:id="rId1"/>
+    <sheet name="mass-transit(durable)" sheetId="1" r:id="rId1"/>
+    <sheet name="easynetq(durable)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -633,9 +634,24 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$A$1:$A$30</c:f>
+              <c:f>'mass-transit(durable)'!$A$1:$A$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -734,7 +750,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$B$1:$B$30</c:f>
+              <c:f>'mass-transit(durable)'!$B$1:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -842,11 +858,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1735538944"/>
-        <c:axId val="-1735538400"/>
+        <c:axId val="1606345232"/>
+        <c:axId val="1606347408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1735538944"/>
+        <c:axId val="1606345232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -889,7 +905,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1735538400"/>
+        <c:crossAx val="1606347408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -897,7 +913,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1735538400"/>
+        <c:axId val="1606347408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -948,9 +964,474 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1735538944"/>
+        <c:crossAx val="1606345232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.0692038495188101E-2"/>
+          <c:y val="2.5428331875182269E-2"/>
+          <c:w val="0.84586351706036744"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'easynetq(durable)'!$A$1:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>270</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'easynetq(durable)'!$B$1:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>11300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8646</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10879</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8547</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9959</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8154</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9815</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9198</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8786</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10335</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9484</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9765</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10177</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10090</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12530</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8260</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8408</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8203</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8401</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9097</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9328</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11842</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10050</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9988</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13432</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8568</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1606338704"/>
+        <c:axId val="1606337072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1606338704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1606337072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1606337072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1606338704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1037,6 +1518,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1534,6 +2055,522 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1571,6 +2608,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>595312</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1853,7 +2925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
@@ -2103,4 +3175,236 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>11300</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>8646</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>10879</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>8547</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>9959</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>8154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <v>9815</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>70</v>
+      </c>
+      <c r="B8">
+        <v>9198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>80</v>
+      </c>
+      <c r="B9">
+        <v>8786</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>90</v>
+      </c>
+      <c r="B10">
+        <v>10335</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>100</v>
+      </c>
+      <c r="B11">
+        <v>9002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>110</v>
+      </c>
+      <c r="B12">
+        <v>9484</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>120</v>
+      </c>
+      <c r="B13">
+        <v>9765</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>130</v>
+      </c>
+      <c r="B14">
+        <v>10177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>150</v>
+      </c>
+      <c r="B15">
+        <v>10090</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>160</v>
+      </c>
+      <c r="B16">
+        <v>12530</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>170</v>
+      </c>
+      <c r="B17">
+        <v>8260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>180</v>
+      </c>
+      <c r="B18">
+        <v>8408</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>190</v>
+      </c>
+      <c r="B19">
+        <v>8203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>200</v>
+      </c>
+      <c r="B20">
+        <v>8401</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>210</v>
+      </c>
+      <c r="B21">
+        <v>9097</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>220</v>
+      </c>
+      <c r="B22">
+        <v>9328</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>230</v>
+      </c>
+      <c r="B23">
+        <v>11842</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>240</v>
+      </c>
+      <c r="B24">
+        <v>10050</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>250</v>
+      </c>
+      <c r="B25">
+        <v>9988</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>260</v>
+      </c>
+      <c r="B26">
+        <v>13432</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>270</v>
+      </c>
+      <c r="B27">
+        <v>8568</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add easynetq non-durable to stats spreadsheet
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="mass-transit(durable)" sheetId="1" r:id="rId1"/>
     <sheet name="easynetq(durable)" sheetId="2" r:id="rId2"/>
+    <sheet name="easynetq(non-durable)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1478,6 +1479,479 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'easynetq(non-durable)'!$A$1:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'easynetq(non-durable)'!$B$1:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>8582</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5719</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5965</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5805</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6391</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6035</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6379</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5309</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6293</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5843</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6714</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6192</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6441</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6601</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5525</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6912</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7181</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5779</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5920</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7805</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4958</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5041</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5635</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5009</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5802</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5193</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5023</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5901</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5177</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1606335984"/>
+        <c:axId val="1604740128"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1606335984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1604740128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1604740128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1606335984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1558,6 +2032,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2075,6 +2589,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2643,6 +3673,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>557211</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3181,7 +4246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -3407,4 +4472,260 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>8582</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>5719</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>5965</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>5805</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>6391</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>6100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <v>6035</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>70</v>
+      </c>
+      <c r="B8">
+        <v>6379</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>80</v>
+      </c>
+      <c r="B9">
+        <v>5309</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>90</v>
+      </c>
+      <c r="B10">
+        <v>6293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>100</v>
+      </c>
+      <c r="B11">
+        <v>5843</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>110</v>
+      </c>
+      <c r="B12">
+        <v>6714</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>120</v>
+      </c>
+      <c r="B13">
+        <v>6192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>130</v>
+      </c>
+      <c r="B14">
+        <v>6441</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>140</v>
+      </c>
+      <c r="B15">
+        <v>6601</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>150</v>
+      </c>
+      <c r="B16">
+        <v>5525</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>160</v>
+      </c>
+      <c r="B17">
+        <v>6912</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>170</v>
+      </c>
+      <c r="B18">
+        <v>7181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>180</v>
+      </c>
+      <c r="B19">
+        <v>5779</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>190</v>
+      </c>
+      <c r="B20">
+        <v>5920</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>200</v>
+      </c>
+      <c r="B21">
+        <v>7805</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>220</v>
+      </c>
+      <c r="B22">
+        <v>4958</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>230</v>
+      </c>
+      <c r="B23">
+        <v>5041</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>240</v>
+      </c>
+      <c r="B24">
+        <v>5635</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>250</v>
+      </c>
+      <c r="B25">
+        <v>5009</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>260</v>
+      </c>
+      <c r="B26">
+        <v>5802</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>270</v>
+      </c>
+      <c r="B27">
+        <v>5193</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>280</v>
+      </c>
+      <c r="B28">
+        <v>5023</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>290</v>
+      </c>
+      <c r="B29">
+        <v>5901</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>300</v>
+      </c>
+      <c r="B30">
+        <v>5177</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add mass-transit non-durable to stats spreadsheet
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="mass-transit(durable)" sheetId="1" r:id="rId1"/>
-    <sheet name="easynetq(durable)" sheetId="2" r:id="rId2"/>
-    <sheet name="easynetq(non-durable)" sheetId="3" r:id="rId3"/>
+    <sheet name="mass-transit(non-durable)" sheetId="4" r:id="rId2"/>
+    <sheet name="easynetq(durable)" sheetId="2" r:id="rId3"/>
+    <sheet name="easynetq(non-durable)" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -756,94 +757,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>49645</c:v>
+                  <c:v>117109</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31654</c:v>
+                  <c:v>90263</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28724</c:v>
+                  <c:v>58283</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23557</c:v>
+                  <c:v>52323</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15230</c:v>
+                  <c:v>41706</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16553</c:v>
+                  <c:v>30749</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19014</c:v>
+                  <c:v>35939</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12873</c:v>
+                  <c:v>35360</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15368</c:v>
+                  <c:v>22411</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12277</c:v>
+                  <c:v>24194</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13163</c:v>
+                  <c:v>21362</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16176</c:v>
+                  <c:v>29888</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13002</c:v>
+                  <c:v>28278</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13942</c:v>
+                  <c:v>30380</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10798</c:v>
+                  <c:v>22789</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11533</c:v>
+                  <c:v>46191</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11131</c:v>
+                  <c:v>26415</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13532</c:v>
+                  <c:v>20355</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10330</c:v>
+                  <c:v>17896</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13317</c:v>
+                  <c:v>19911</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8964</c:v>
+                  <c:v>20604</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>11377</c:v>
+                  <c:v>26008</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9506</c:v>
+                  <c:v>18625</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10404</c:v>
+                  <c:v>18680</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>10937</c:v>
+                  <c:v>17840</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12093</c:v>
+                  <c:v>17402</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>16434</c:v>
+                  <c:v>20494</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8975</c:v>
+                  <c:v>37684</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>11743</c:v>
+                  <c:v>18240</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7679</c:v>
+                  <c:v>17378</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -859,11 +860,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1606345232"/>
-        <c:axId val="1606347408"/>
+        <c:axId val="-877894912"/>
+        <c:axId val="-877887840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1606345232"/>
+        <c:axId val="-877894912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -906,7 +907,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1606347408"/>
+        <c:crossAx val="-877887840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -914,7 +915,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1606347408"/>
+        <c:axId val="-877887840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -965,7 +966,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1606345232"/>
+        <c:crossAx val="-877894912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1015,6 +1016,467 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'mass-transit(non-durable)'!$A$1:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>280</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'mass-transit(non-durable)'!$B$1:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>13091</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11656</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10897</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10962</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10991</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10637</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10794</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10637</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12625</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10924</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12373</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8543</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19483</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13976</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12618</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10887</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11438</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32910</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30911</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22150</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9255</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>60676</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11774</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9107</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33270</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>59886</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>36840</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>60145</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1117115968"/>
+        <c:axId val="-1017386000"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1117115968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1017386000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1017386000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1117115968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1307,11 +1769,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1606338704"/>
-        <c:axId val="1606337072"/>
+        <c:axId val="-877892736"/>
+        <c:axId val="-1017383280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1606338704"/>
+        <c:axId val="-877892736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1368,12 +1830,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1606337072"/>
+        <c:crossAx val="-1017383280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1606337072"/>
+        <c:axId val="-1017383280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,7 +1892,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1606338704"/>
+        <c:crossAx val="-877892736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1479,7 +1941,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1780,11 +2242,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1606335984"/>
-        <c:axId val="1604740128"/>
+        <c:axId val="-880858144"/>
+        <c:axId val="-792122736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1606335984"/>
+        <c:axId val="-880858144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1841,12 +2303,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1604740128"/>
+        <c:crossAx val="-792122736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1604740128"/>
+        <c:axId val="-792122736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1903,7 +2365,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1606335984"/>
+        <c:crossAx val="-880858144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2072,6 +2534,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3105,6 +3607,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3660,6 +4678,41 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>595312</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
@@ -3690,7 +4743,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3990,8 +5043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4001,7 +5054,7 @@
         <v>10</v>
       </c>
       <c r="B1">
-        <v>49645</v>
+        <v>117109</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4009,7 +5062,7 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <v>31654</v>
+        <v>90263</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4017,7 +5070,7 @@
         <v>30</v>
       </c>
       <c r="B3">
-        <v>28724</v>
+        <v>58283</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4025,7 +5078,7 @@
         <v>40</v>
       </c>
       <c r="B4">
-        <v>23557</v>
+        <v>52323</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -4033,7 +5086,7 @@
         <v>50</v>
       </c>
       <c r="B5">
-        <v>15230</v>
+        <v>41706</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4041,7 +5094,7 @@
         <v>60</v>
       </c>
       <c r="B6">
-        <v>16553</v>
+        <v>30749</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -4049,7 +5102,7 @@
         <v>70</v>
       </c>
       <c r="B7">
-        <v>19014</v>
+        <v>35939</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -4057,7 +5110,7 @@
         <v>80</v>
       </c>
       <c r="B8">
-        <v>12873</v>
+        <v>35360</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4065,7 +5118,7 @@
         <v>90</v>
       </c>
       <c r="B9">
-        <v>15368</v>
+        <v>22411</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -4073,7 +5126,7 @@
         <v>100</v>
       </c>
       <c r="B10">
-        <v>12277</v>
+        <v>24194</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -4081,7 +5134,7 @@
         <v>110</v>
       </c>
       <c r="B11">
-        <v>13163</v>
+        <v>21362</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -4089,7 +5142,7 @@
         <v>120</v>
       </c>
       <c r="B12">
-        <v>16176</v>
+        <v>29888</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -4097,7 +5150,7 @@
         <v>130</v>
       </c>
       <c r="B13">
-        <v>13002</v>
+        <v>28278</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -4105,7 +5158,7 @@
         <v>140</v>
       </c>
       <c r="B14">
-        <v>13942</v>
+        <v>30380</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -4113,7 +5166,7 @@
         <v>150</v>
       </c>
       <c r="B15">
-        <v>10798</v>
+        <v>22789</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -4121,7 +5174,7 @@
         <v>160</v>
       </c>
       <c r="B16">
-        <v>11533</v>
+        <v>46191</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -4129,7 +5182,7 @@
         <v>170</v>
       </c>
       <c r="B17">
-        <v>11131</v>
+        <v>26415</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -4137,7 +5190,7 @@
         <v>180</v>
       </c>
       <c r="B18">
-        <v>13532</v>
+        <v>20355</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -4145,7 +5198,7 @@
         <v>190</v>
       </c>
       <c r="B19">
-        <v>10330</v>
+        <v>17896</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -4153,7 +5206,7 @@
         <v>200</v>
       </c>
       <c r="B20">
-        <v>13317</v>
+        <v>19911</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -4161,7 +5214,7 @@
         <v>210</v>
       </c>
       <c r="B21">
-        <v>8964</v>
+        <v>20604</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -4169,7 +5222,7 @@
         <v>220</v>
       </c>
       <c r="B22">
-        <v>11377</v>
+        <v>26008</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -4177,7 +5230,7 @@
         <v>230</v>
       </c>
       <c r="B23">
-        <v>9506</v>
+        <v>18625</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -4185,7 +5238,7 @@
         <v>240</v>
       </c>
       <c r="B24">
-        <v>10404</v>
+        <v>18680</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -4193,7 +5246,7 @@
         <v>250</v>
       </c>
       <c r="B25">
-        <v>10937</v>
+        <v>17840</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -4201,7 +5254,7 @@
         <v>260</v>
       </c>
       <c r="B26">
-        <v>12093</v>
+        <v>17402</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -4209,7 +5262,7 @@
         <v>270</v>
       </c>
       <c r="B27">
-        <v>16434</v>
+        <v>20494</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -4217,7 +5270,7 @@
         <v>280</v>
       </c>
       <c r="B28">
-        <v>8975</v>
+        <v>37684</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -4225,7 +5278,7 @@
         <v>290</v>
       </c>
       <c r="B29">
-        <v>11743</v>
+        <v>18240</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -4233,7 +5286,7 @@
         <v>300</v>
       </c>
       <c r="B30">
-        <v>7679</v>
+        <v>17378</v>
       </c>
     </row>
   </sheetData>
@@ -4243,6 +5296,246 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V30" sqref="V30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>10</v>
+      </c>
+      <c r="B1">
+        <v>13091</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>11656</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>10897</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>40</v>
+      </c>
+      <c r="B4">
+        <v>10962</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>10991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>10637</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>70</v>
+      </c>
+      <c r="B7">
+        <v>10794</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>80</v>
+      </c>
+      <c r="B8">
+        <v>10637</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>90</v>
+      </c>
+      <c r="B9">
+        <v>12625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>100</v>
+      </c>
+      <c r="B10">
+        <v>10924</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>110</v>
+      </c>
+      <c r="B11">
+        <v>12373</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>120</v>
+      </c>
+      <c r="B12">
+        <v>8543</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>130</v>
+      </c>
+      <c r="B13">
+        <v>19483</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>140</v>
+      </c>
+      <c r="B14">
+        <v>13976</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>150</v>
+      </c>
+      <c r="B15">
+        <v>12618</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>160</v>
+      </c>
+      <c r="B16">
+        <v>10887</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>170</v>
+      </c>
+      <c r="B17">
+        <v>11438</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>180</v>
+      </c>
+      <c r="B18">
+        <v>32910</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>190</v>
+      </c>
+      <c r="B19">
+        <v>30911</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>200</v>
+      </c>
+      <c r="B20">
+        <v>22150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>210</v>
+      </c>
+      <c r="B21">
+        <v>9255</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>220</v>
+      </c>
+      <c r="B22">
+        <v>60676</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>230</v>
+      </c>
+      <c r="B23">
+        <v>11774</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>240</v>
+      </c>
+      <c r="B24">
+        <v>9107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>250</v>
+      </c>
+      <c r="B25">
+        <v>33270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>260</v>
+      </c>
+      <c r="B26">
+        <v>59886</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>270</v>
+      </c>
+      <c r="B27">
+        <v>36840</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>280</v>
+      </c>
+      <c r="B28">
+        <v>60145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
@@ -4474,11 +5767,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>

</xml_diff>